<commit_message>
Updated index.html and server.js
</commit_message>
<xml_diff>
--- a/registrations.xlsx
+++ b/registrations.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F134EC7A-181C-4FEA-A8E0-F6E7370CD55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Registrations" state="visible" r:id="rId4"/>
+    <sheet name="Registrations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -28,9 +32,6 @@
     <t>TshirtSize</t>
   </si>
   <si>
-    <t>OrderId</t>
-  </si>
-  <si>
     <t>PaymentId</t>
   </si>
   <si>
@@ -38,19 +39,22 @@
   </si>
   <si>
     <t>PaymentStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lower size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,11 +417,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,20 +443,20 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>